<commit_message>
LinguaF plots and statistics added
</commit_message>
<xml_diff>
--- a/Review files/qald9_test_set_review_table.xlsx
+++ b/Review files/qald9_test_set_review_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi\Desktop\Work\QALD9ES\Repo\QALD9-ES\Review files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D8522-6BFC-44CB-B442-D94938D756F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71DA56C-D82F-482C-A1BE-D09933EE4575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="950">
   <si>
     <t>id</t>
   </si>
@@ -2864,6 +2864,12 @@
   </si>
   <si>
     <t>página de Web,  empresas,  empleados,  más de 500000</t>
+  </si>
+  <si>
+    <t>¿En qué rutas de senderismo del Gran Cañón no hay riesgo de inundaciones repentinas?</t>
+  </si>
+  <si>
+    <t>rutas senderismo,  Gran Cañón,  no riesgo,  inundaciones repentinas</t>
   </si>
 </sst>
 </file>
@@ -3265,11 +3271,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L150" sqref="L150"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K147" sqref="K147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7481,11 +7487,23 @@
       <c r="C147" t="s">
         <v>458</v>
       </c>
+      <c r="D147" t="s">
+        <v>948</v>
+      </c>
       <c r="E147" t="s">
         <v>608</v>
       </c>
       <c r="F147" t="s">
         <v>758</v>
+      </c>
+      <c r="G147" t="s">
+        <v>949</v>
+      </c>
+      <c r="K147" t="s">
+        <v>763</v>
+      </c>
+      <c r="M147" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
@@ -7605,11 +7623,6 @@
       </c>
       <c r="M151" t="s">
         <v>763</v>
-      </c>
-    </row>
-    <row r="1048576" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D1048576" t="s">
-        <v>920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QALD9-ES and updated QALD9 Generated with native translations
</commit_message>
<xml_diff>
--- a/Review files/qald9_test_set_review_table.xlsx
+++ b/Review files/qald9_test_set_review_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi\Desktop\Work\QALD9ES\Repo\QALD9-ES\Review files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71DA56C-D82F-482C-A1BE-D09933EE4575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCF7BBA-32EB-4581-87C8-5650F860421F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="956">
   <si>
     <t>id</t>
   </si>
@@ -2452,12 +2452,6 @@
     <t>río, más largo, China</t>
   </si>
   <si>
-    <t>¿Cuál es el prefijo de Berlín?</t>
-  </si>
-  <si>
-    <t>prefijo,  Berlín</t>
-  </si>
-  <si>
     <t>¿Cuántos científicos se han graduado de una Universidad de la Ivy League?</t>
   </si>
   <si>
@@ -2512,9 +2506,6 @@
     <t>Universidad Libre de Ámsterdam,  estudiantes</t>
   </si>
   <si>
-    <t>¿Cuántos son los ingresos generados por IBM?</t>
-  </si>
-  <si>
     <t xml:space="preserve">ingresos, IBM </t>
   </si>
   <si>
@@ -2569,9 +2560,6 @@
     <t>muerte, creador, Drácula</t>
   </si>
   <si>
-    <t>¿Quién creó la Wikipedia en inglés?</t>
-  </si>
-  <si>
     <t xml:space="preserve">creador, Inglés, Wikipedia </t>
   </si>
   <si>
@@ -2605,9 +2593,6 @@
     <t>Lago Chiem, profundidad</t>
   </si>
   <si>
-    <t>¿Qué empresas operan tanto en la industria aeroespacial como en la industria médica?</t>
-  </si>
-  <si>
     <t>empresas,  industria aeroespacial, industria médica</t>
   </si>
   <si>
@@ -2662,12 +2647,6 @@
     <t>Ramones,  lado B</t>
   </si>
   <si>
-    <t>apodo,  Scarface</t>
-  </si>
-  <si>
-    <t>¿Dónde se encuentra el Fort Knox?</t>
-  </si>
-  <si>
     <t>Fort Knox, ubicación</t>
   </si>
   <si>
@@ -2728,9 +2707,6 @@
     <t>políticos, casados, alemán</t>
   </si>
   <si>
-    <t>¿Es el nombre de la esposa del presidente Obama Michelle?</t>
-  </si>
-  <si>
     <t xml:space="preserve">esposa,  presidente, Obama,  nombre, Michelle </t>
   </si>
   <si>
@@ -2764,12 +2740,6 @@
     <t>sitio web oficial ,   actores , programa de televisión, Charmed</t>
   </si>
   <si>
-    <t>¿Qué librerías fueron fundadas antes de 1400?</t>
-  </si>
-  <si>
-    <t>librerías, fundadas,  antes de 1400</t>
-  </si>
-  <si>
     <t>¿Qué islas pertenecientes a las islas Frisias son parte de los Países Bajos?</t>
   </si>
   <si>
@@ -2815,9 +2785,6 @@
     <t>Cat Stevens,  instrumentos,  toca</t>
   </si>
   <si>
-    <t>¿Quién era llamado Rodzilla?</t>
-  </si>
-  <si>
     <t>apodo,  Rodzilla</t>
   </si>
   <si>
@@ -2836,12 +2803,6 @@
     <t xml:space="preserve">más grande, estado , Estados Unidos </t>
   </si>
   <si>
-    <t>¿Cómo se llamaban las tres naves utilizadas por Colón?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tres naves ,   nombre ,   Colón </t>
-  </si>
-  <si>
     <t>programa de viajero frecuente, más aerolíneas</t>
   </si>
   <si>
@@ -2870,6 +2831,63 @@
   </si>
   <si>
     <t>rutas senderismo,  Gran Cañón,  no riesgo,  inundaciones repentinas</t>
+  </si>
+  <si>
+    <t>Dame la página web de Forbes.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código de área de Berlín?</t>
+  </si>
+  <si>
+    <t>código de área,  Berlín</t>
+  </si>
+  <si>
+    <t>¿Cuándo le dispararon a Carlo Giuliani?</t>
+  </si>
+  <si>
+    <t>¿Cuáles son los ingresos generados por IBM?</t>
+  </si>
+  <si>
+    <t>¿Quién creó Wikipedia en inglés?</t>
+  </si>
+  <si>
+    <t>¿Qué empresas trabajan tanto en la industria aeroespacial como en la medicina?</t>
+  </si>
+  <si>
+    <t>¿Quién se llamaba Caracortada?</t>
+  </si>
+  <si>
+    <t>apodo,  Caracortada</t>
+  </si>
+  <si>
+    <t>¿Qué hijas de condes británicos murieron en el mismo lugar donde nacieron?</t>
+  </si>
+  <si>
+    <t>hijas,  condes británicos,  murieron,  lugar de nacimiento</t>
+  </si>
+  <si>
+    <t>¿Dónde se encuentra ubicado Fort Knox?</t>
+  </si>
+  <si>
+    <t>¿La esposa del presidente Obama se llama Michelle?</t>
+  </si>
+  <si>
+    <t>¿Cuándo falleció Muhammad?</t>
+  </si>
+  <si>
+    <t>¿Quién era conocido como Rodzilla?</t>
+  </si>
+  <si>
+    <t>¿Cómo se llamaban los tres barcos utilizados por Colón?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tres barcos ,   nombre ,   Colón </t>
+  </si>
+  <si>
+    <t>¿Qué librerías fueron construidas antes de 1400?</t>
+  </si>
+  <si>
+    <t>librerías, construidas,  antes de 1400</t>
   </si>
 </sst>
 </file>
@@ -3273,19 +3291,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K147" sqref="K147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.140625" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="81.28515625" customWidth="1"/>
+    <col min="4" max="4" width="97.42578125" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" customWidth="1"/>
     <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3630,7 +3648,7 @@
         <v>623</v>
       </c>
       <c r="G12" t="s">
-        <v>940</v>
+        <v>927</v>
       </c>
       <c r="K12" t="s">
         <v>763</v>
@@ -4108,7 +4126,7 @@
         <v>341</v>
       </c>
       <c r="D29" t="s">
-        <v>341</v>
+        <v>937</v>
       </c>
       <c r="E29" t="s">
         <v>490</v>
@@ -4119,7 +4137,7 @@
       <c r="G29" t="s">
         <v>640</v>
       </c>
-      <c r="N29" t="s">
+      <c r="H29" t="s">
         <v>763</v>
       </c>
     </row>
@@ -4508,7 +4526,7 @@
         <v>355</v>
       </c>
       <c r="D43" t="s">
-        <v>810</v>
+        <v>938</v>
       </c>
       <c r="E43" t="s">
         <v>504</v>
@@ -4517,12 +4535,15 @@
         <v>654</v>
       </c>
       <c r="G43" t="s">
-        <v>811</v>
+        <v>939</v>
       </c>
       <c r="K43" t="s">
         <v>763</v>
       </c>
       <c r="L43" t="s">
+        <v>763</v>
+      </c>
+      <c r="M43" t="s">
         <v>763</v>
       </c>
     </row>
@@ -4537,7 +4558,7 @@
         <v>356</v>
       </c>
       <c r="D44" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E44" t="s">
         <v>505</v>
@@ -4546,7 +4567,7 @@
         <v>655</v>
       </c>
       <c r="G44" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="H44" t="s">
         <v>763</v>
@@ -4627,7 +4648,7 @@
         <v>658</v>
       </c>
       <c r="G47" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="K47" t="s">
         <v>763</v>
@@ -4659,7 +4680,7 @@
         <v>659</v>
       </c>
       <c r="G48" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="N48" t="s">
         <v>763</v>
@@ -4676,7 +4697,7 @@
         <v>361</v>
       </c>
       <c r="D49" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E49" t="s">
         <v>510</v>
@@ -4685,7 +4706,7 @@
         <v>660</v>
       </c>
       <c r="G49" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="K49" t="s">
         <v>763</v>
@@ -4705,7 +4726,7 @@
         <v>362</v>
       </c>
       <c r="D50" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="E50" t="s">
         <v>511</v>
@@ -4734,7 +4755,7 @@
         <v>363</v>
       </c>
       <c r="D51" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="E51" t="s">
         <v>512</v>
@@ -4743,7 +4764,7 @@
         <v>662</v>
       </c>
       <c r="G51" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="K51" t="s">
         <v>763</v>
@@ -4772,7 +4793,7 @@
         <v>663</v>
       </c>
       <c r="G52" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="K52" t="s">
         <v>763</v>
@@ -4792,7 +4813,7 @@
         <v>365</v>
       </c>
       <c r="D53" t="s">
-        <v>365</v>
+        <v>940</v>
       </c>
       <c r="E53" t="s">
         <v>514</v>
@@ -4803,7 +4824,7 @@
       <c r="G53" t="s">
         <v>664</v>
       </c>
-      <c r="N53" t="s">
+      <c r="M53" t="s">
         <v>763</v>
       </c>
     </row>
@@ -4818,7 +4839,7 @@
         <v>366</v>
       </c>
       <c r="D54" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="E54" t="s">
         <v>515</v>
@@ -4844,7 +4865,7 @@
         <v>367</v>
       </c>
       <c r="D55" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="E55" t="s">
         <v>516</v>
@@ -4853,7 +4874,7 @@
         <v>666</v>
       </c>
       <c r="G55" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="J55" t="s">
         <v>763</v>
@@ -4876,7 +4897,7 @@
         <v>368</v>
       </c>
       <c r="D56" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="E56" t="s">
         <v>517</v>
@@ -4885,7 +4906,7 @@
         <v>667</v>
       </c>
       <c r="G56" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="K56" t="s">
         <v>763</v>
@@ -4940,7 +4961,7 @@
         <v>669</v>
       </c>
       <c r="G58" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="K58" t="s">
         <v>763</v>
@@ -5012,7 +5033,7 @@
         <v>373</v>
       </c>
       <c r="D61" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E61" t="s">
         <v>522</v>
@@ -5021,7 +5042,7 @@
         <v>672</v>
       </c>
       <c r="G61" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="K61" t="s">
         <v>763</v>
@@ -5041,7 +5062,7 @@
         <v>374</v>
       </c>
       <c r="D62" t="s">
-        <v>830</v>
+        <v>941</v>
       </c>
       <c r="E62" t="s">
         <v>523</v>
@@ -5050,7 +5071,7 @@
         <v>673</v>
       </c>
       <c r="G62" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="H62" t="s">
         <v>763</v>
@@ -5122,7 +5143,7 @@
         <v>377</v>
       </c>
       <c r="D65" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="E65" t="s">
         <v>526</v>
@@ -5131,7 +5152,7 @@
         <v>676</v>
       </c>
       <c r="G65" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="J65" t="s">
         <v>763</v>
@@ -5180,7 +5201,7 @@
         <v>379</v>
       </c>
       <c r="D67" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="E67" t="s">
         <v>528</v>
@@ -5232,7 +5253,7 @@
         <v>381</v>
       </c>
       <c r="D69" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="E69" t="s">
         <v>530</v>
@@ -5241,7 +5262,7 @@
         <v>680</v>
       </c>
       <c r="G69" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="K69" t="s">
         <v>763</v>
@@ -5261,7 +5282,7 @@
         <v>382</v>
       </c>
       <c r="D70" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="E70" t="s">
         <v>531</v>
@@ -5270,7 +5291,7 @@
         <v>681</v>
       </c>
       <c r="G70" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="K70" t="s">
         <v>763</v>
@@ -5299,7 +5320,7 @@
         <v>682</v>
       </c>
       <c r="G71" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="L71" t="s">
         <v>763</v>
@@ -5319,7 +5340,7 @@
         <v>384</v>
       </c>
       <c r="D72" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="E72" t="s">
         <v>533</v>
@@ -5345,7 +5366,7 @@
         <v>385</v>
       </c>
       <c r="D73" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="E73" t="s">
         <v>534</v>
@@ -5354,7 +5375,7 @@
         <v>684</v>
       </c>
       <c r="G73" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="L73" t="s">
         <v>763</v>
@@ -5371,7 +5392,7 @@
         <v>386</v>
       </c>
       <c r="D74" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="E74" t="s">
         <v>535</v>
@@ -5406,7 +5427,7 @@
         <v>686</v>
       </c>
       <c r="G75" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="K75" t="s">
         <v>763</v>
@@ -5423,7 +5444,7 @@
         <v>388</v>
       </c>
       <c r="D76" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="E76" t="s">
         <v>537</v>
@@ -5432,7 +5453,7 @@
         <v>687</v>
       </c>
       <c r="G76" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="I76" t="s">
         <v>763</v>
@@ -5458,7 +5479,7 @@
         <v>389</v>
       </c>
       <c r="D77" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="E77" t="s">
         <v>538</v>
@@ -5467,7 +5488,7 @@
         <v>688</v>
       </c>
       <c r="G77" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="L77" t="s">
         <v>763</v>
@@ -5484,7 +5505,7 @@
         <v>390</v>
       </c>
       <c r="D78" t="s">
-        <v>849</v>
+        <v>942</v>
       </c>
       <c r="E78" t="s">
         <v>539</v>
@@ -5493,7 +5514,7 @@
         <v>689</v>
       </c>
       <c r="G78" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="H78" t="s">
         <v>763</v>
@@ -5502,6 +5523,9 @@
         <v>763</v>
       </c>
       <c r="L78" t="s">
+        <v>763</v>
+      </c>
+      <c r="M78" t="s">
         <v>763</v>
       </c>
     </row>
@@ -5516,7 +5540,7 @@
         <v>391</v>
       </c>
       <c r="D79" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="E79" t="s">
         <v>540</v>
@@ -5525,7 +5549,7 @@
         <v>690</v>
       </c>
       <c r="G79" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="K79" t="s">
         <v>763</v>
@@ -5545,7 +5569,7 @@
         <v>392</v>
       </c>
       <c r="D80" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="E80" t="s">
         <v>541</v>
@@ -5554,7 +5578,7 @@
         <v>691</v>
       </c>
       <c r="G80" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="K80" t="s">
         <v>763</v>
@@ -5574,7 +5598,7 @@
         <v>393</v>
       </c>
       <c r="D81" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="E81" t="s">
         <v>542</v>
@@ -5583,7 +5607,7 @@
         <v>692</v>
       </c>
       <c r="G81" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="H81" t="s">
         <v>763</v>
@@ -5609,7 +5633,7 @@
         <v>394</v>
       </c>
       <c r="D82" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="E82" t="s">
         <v>543</v>
@@ -5618,7 +5642,7 @@
         <v>693</v>
       </c>
       <c r="G82" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="K82" t="s">
         <v>763</v>
@@ -5638,7 +5662,7 @@
         <v>395</v>
       </c>
       <c r="D83" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="E83" t="s">
         <v>544</v>
@@ -5647,7 +5671,7 @@
         <v>694</v>
       </c>
       <c r="G83" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="H83" t="s">
         <v>763</v>
@@ -5673,7 +5697,7 @@
         <v>396</v>
       </c>
       <c r="D84" t="s">
-        <v>861</v>
+        <v>943</v>
       </c>
       <c r="E84" t="s">
         <v>545</v>
@@ -5682,7 +5706,7 @@
         <v>695</v>
       </c>
       <c r="G84" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="K84" t="s">
         <v>763</v>
@@ -5737,7 +5761,7 @@
         <v>697</v>
       </c>
       <c r="G86" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="K86" t="s">
         <v>763</v>
@@ -5766,7 +5790,7 @@
         <v>698</v>
       </c>
       <c r="G87" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="I87" t="s">
         <v>763</v>
@@ -5815,7 +5839,7 @@
         <v>401</v>
       </c>
       <c r="D89" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="E89" t="s">
         <v>550</v>
@@ -5841,7 +5865,7 @@
         <v>402</v>
       </c>
       <c r="D90" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="E90" t="s">
         <v>551</v>
@@ -5850,7 +5874,7 @@
         <v>701</v>
       </c>
       <c r="G90" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="I90" t="s">
         <v>763</v>
@@ -5908,7 +5932,7 @@
         <v>703</v>
       </c>
       <c r="G92" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="K92" t="s">
         <v>763</v>
@@ -5928,7 +5952,7 @@
         <v>405</v>
       </c>
       <c r="D93" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="E93" t="s">
         <v>554</v>
@@ -5954,7 +5978,7 @@
         <v>406</v>
       </c>
       <c r="D94" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="E94" t="s">
         <v>555</v>
@@ -5963,7 +5987,7 @@
         <v>705</v>
       </c>
       <c r="G94" t="s">
-        <v>941</v>
+        <v>928</v>
       </c>
       <c r="H94" t="s">
         <v>763</v>
@@ -5986,7 +6010,7 @@
         <v>407</v>
       </c>
       <c r="D95" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="E95" t="s">
         <v>556</v>
@@ -6012,7 +6036,7 @@
         <v>408</v>
       </c>
       <c r="D96" t="s">
-        <v>942</v>
+        <v>929</v>
       </c>
       <c r="E96" t="s">
         <v>557</v>
@@ -6021,7 +6045,7 @@
         <v>707</v>
       </c>
       <c r="G96" t="s">
-        <v>943</v>
+        <v>930</v>
       </c>
       <c r="K96" t="s">
         <v>763</v>
@@ -6070,7 +6094,7 @@
         <v>410</v>
       </c>
       <c r="D98" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="E98" t="s">
         <v>559</v>
@@ -6079,7 +6103,7 @@
         <v>709</v>
       </c>
       <c r="G98" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="I98" t="s">
         <v>763</v>
@@ -6105,7 +6129,7 @@
         <v>411</v>
       </c>
       <c r="D99" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
       <c r="E99" t="s">
         <v>560</v>
@@ -6114,7 +6138,7 @@
         <v>710</v>
       </c>
       <c r="G99" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="I99" t="s">
         <v>763</v>
@@ -6131,10 +6155,10 @@
         <v>262</v>
       </c>
       <c r="C100" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="D100" t="s">
-        <v>944</v>
+        <v>931</v>
       </c>
       <c r="E100" t="s">
         <v>561</v>
@@ -6143,7 +6167,7 @@
         <v>711</v>
       </c>
       <c r="G100" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="K100" t="s">
         <v>763</v>
@@ -6163,7 +6187,7 @@
         <v>412</v>
       </c>
       <c r="D101" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
       <c r="E101" t="s">
         <v>562</v>
@@ -6172,7 +6196,7 @@
         <v>712</v>
       </c>
       <c r="G101" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="K101" t="s">
         <v>763</v>
@@ -6192,7 +6216,7 @@
         <v>413</v>
       </c>
       <c r="D102" t="s">
-        <v>413</v>
+        <v>944</v>
       </c>
       <c r="E102" t="s">
         <v>563</v>
@@ -6201,7 +6225,10 @@
         <v>713</v>
       </c>
       <c r="G102" t="s">
-        <v>880</v>
+        <v>945</v>
+      </c>
+      <c r="I102" t="s">
+        <v>763</v>
       </c>
       <c r="K102" t="s">
         <v>763</v>
@@ -6244,7 +6271,7 @@
         <v>415</v>
       </c>
       <c r="D104" t="s">
-        <v>881</v>
+        <v>948</v>
       </c>
       <c r="E104" t="s">
         <v>565</v>
@@ -6253,12 +6280,18 @@
         <v>715</v>
       </c>
       <c r="G104" t="s">
-        <v>882</v>
+        <v>875</v>
+      </c>
+      <c r="H104" t="s">
+        <v>763</v>
       </c>
       <c r="K104" t="s">
         <v>763</v>
       </c>
       <c r="L104" t="s">
+        <v>763</v>
+      </c>
+      <c r="M104" t="s">
         <v>763</v>
       </c>
     </row>
@@ -6273,7 +6306,7 @@
         <v>416</v>
       </c>
       <c r="D105" t="s">
-        <v>416</v>
+        <v>946</v>
       </c>
       <c r="E105" t="s">
         <v>566</v>
@@ -6282,9 +6315,9 @@
         <v>716</v>
       </c>
       <c r="G105" t="s">
-        <v>716</v>
-      </c>
-      <c r="N105" t="s">
+        <v>947</v>
+      </c>
+      <c r="M105" t="s">
         <v>763</v>
       </c>
     </row>
@@ -6308,7 +6341,7 @@
         <v>717</v>
       </c>
       <c r="G106" t="s">
-        <v>883</v>
+        <v>876</v>
       </c>
       <c r="K106" t="s">
         <v>763</v>
@@ -6328,7 +6361,7 @@
         <v>418</v>
       </c>
       <c r="D107" t="s">
-        <v>884</v>
+        <v>877</v>
       </c>
       <c r="E107" t="s">
         <v>568</v>
@@ -6337,7 +6370,7 @@
         <v>718</v>
       </c>
       <c r="G107" t="s">
-        <v>885</v>
+        <v>878</v>
       </c>
       <c r="I107" t="s">
         <v>763</v>
@@ -6383,7 +6416,7 @@
         <v>420</v>
       </c>
       <c r="D109" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="E109" t="s">
         <v>570</v>
@@ -6392,7 +6425,7 @@
         <v>720</v>
       </c>
       <c r="G109" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="K109" t="s">
         <v>763</v>
@@ -6412,7 +6445,7 @@
         <v>421</v>
       </c>
       <c r="D110" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="E110" t="s">
         <v>571</v>
@@ -6441,7 +6474,7 @@
         <v>422</v>
       </c>
       <c r="D111" t="s">
-        <v>889</v>
+        <v>882</v>
       </c>
       <c r="E111" t="s">
         <v>572</v>
@@ -6450,7 +6483,7 @@
         <v>722</v>
       </c>
       <c r="G111" t="s">
-        <v>890</v>
+        <v>883</v>
       </c>
       <c r="K111" t="s">
         <v>763</v>
@@ -6473,7 +6506,7 @@
         <v>423</v>
       </c>
       <c r="D112" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="E112" t="s">
         <v>573</v>
@@ -6482,7 +6515,7 @@
         <v>723</v>
       </c>
       <c r="G112" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="I112" t="s">
         <v>763</v>
@@ -6508,7 +6541,7 @@
         <v>424</v>
       </c>
       <c r="D113" t="s">
-        <v>945</v>
+        <v>932</v>
       </c>
       <c r="E113" t="s">
         <v>574</v>
@@ -6517,7 +6550,7 @@
         <v>724</v>
       </c>
       <c r="G113" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="K113" t="s">
         <v>763</v>
@@ -6537,7 +6570,7 @@
         <v>425</v>
       </c>
       <c r="D114" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="E114" t="s">
         <v>575</v>
@@ -6546,7 +6579,7 @@
         <v>725</v>
       </c>
       <c r="G114" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="K114" t="s">
         <v>763</v>
@@ -6575,7 +6608,7 @@
         <v>726</v>
       </c>
       <c r="G115" t="s">
-        <v>946</v>
+        <v>933</v>
       </c>
       <c r="K115" t="s">
         <v>763</v>
@@ -6595,7 +6628,7 @@
         <v>427</v>
       </c>
       <c r="D116" t="s">
-        <v>896</v>
+        <v>889</v>
       </c>
       <c r="E116" t="s">
         <v>577</v>
@@ -6604,7 +6637,7 @@
         <v>727</v>
       </c>
       <c r="G116" t="s">
-        <v>897</v>
+        <v>890</v>
       </c>
       <c r="H116" t="s">
         <v>763</v>
@@ -6627,7 +6660,7 @@
         <v>428</v>
       </c>
       <c r="D117" t="s">
-        <v>898</v>
+        <v>891</v>
       </c>
       <c r="E117" t="s">
         <v>578</v>
@@ -6636,7 +6669,7 @@
         <v>728</v>
       </c>
       <c r="G117" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="I117" t="s">
         <v>763</v>
@@ -6659,7 +6692,7 @@
         <v>429</v>
       </c>
       <c r="D118" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="E118" t="s">
         <v>579</v>
@@ -6668,7 +6701,7 @@
         <v>729</v>
       </c>
       <c r="G118" t="s">
-        <v>901</v>
+        <v>894</v>
       </c>
       <c r="J118" t="s">
         <v>763</v>
@@ -6714,7 +6747,7 @@
         <v>431</v>
       </c>
       <c r="D120" t="s">
-        <v>902</v>
+        <v>949</v>
       </c>
       <c r="E120" t="s">
         <v>581</v>
@@ -6723,7 +6756,7 @@
         <v>731</v>
       </c>
       <c r="G120" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="H120" t="s">
         <v>763</v>
@@ -6772,7 +6805,7 @@
         <v>433</v>
       </c>
       <c r="D122" t="s">
-        <v>433</v>
+        <v>950</v>
       </c>
       <c r="E122" t="s">
         <v>583</v>
@@ -6781,12 +6814,12 @@
         <v>733</v>
       </c>
       <c r="G122" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="K122" t="s">
         <v>763</v>
       </c>
-      <c r="N122" t="s">
+      <c r="M122" t="s">
         <v>763</v>
       </c>
     </row>
@@ -6801,7 +6834,7 @@
         <v>434</v>
       </c>
       <c r="D123" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="E123" t="s">
         <v>584</v>
@@ -6810,7 +6843,7 @@
         <v>734</v>
       </c>
       <c r="G123" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="K123" t="s">
         <v>763</v>
@@ -6830,7 +6863,7 @@
         <v>435</v>
       </c>
       <c r="D124" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="E124" t="s">
         <v>585</v>
@@ -6859,7 +6892,7 @@
         <v>436</v>
       </c>
       <c r="D125" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="E125" t="s">
         <v>586</v>
@@ -6868,7 +6901,7 @@
         <v>736</v>
       </c>
       <c r="G125" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="K125" t="s">
         <v>763</v>
@@ -6888,7 +6921,7 @@
         <v>437</v>
       </c>
       <c r="D126" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="E126" t="s">
         <v>587</v>
@@ -6897,7 +6930,7 @@
         <v>737</v>
       </c>
       <c r="G126" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="H126" t="s">
         <v>763</v>
@@ -6917,7 +6950,7 @@
         <v>438</v>
       </c>
       <c r="D127" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="E127" t="s">
         <v>588</v>
@@ -6926,7 +6959,7 @@
         <v>738</v>
       </c>
       <c r="G127" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="I127" t="s">
         <v>763</v>
@@ -6975,7 +7008,7 @@
         <v>440</v>
       </c>
       <c r="D129" t="s">
-        <v>914</v>
+        <v>954</v>
       </c>
       <c r="E129" t="s">
         <v>590</v>
@@ -6984,7 +7017,7 @@
         <v>740</v>
       </c>
       <c r="G129" t="s">
-        <v>915</v>
+        <v>955</v>
       </c>
       <c r="K129" t="s">
         <v>763</v>
@@ -7004,7 +7037,7 @@
         <v>441</v>
       </c>
       <c r="D130" t="s">
-        <v>916</v>
+        <v>906</v>
       </c>
       <c r="E130" t="s">
         <v>591</v>
@@ -7013,7 +7046,7 @@
         <v>741</v>
       </c>
       <c r="G130" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="I130" t="s">
         <v>763</v>
@@ -7036,7 +7069,7 @@
         <v>442</v>
       </c>
       <c r="D131" t="s">
-        <v>918</v>
+        <v>908</v>
       </c>
       <c r="E131" t="s">
         <v>592</v>
@@ -7088,7 +7121,7 @@
         <v>444</v>
       </c>
       <c r="D133" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
       <c r="E133" t="s">
         <v>594</v>
@@ -7120,7 +7153,7 @@
         <v>445</v>
       </c>
       <c r="D134" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="E134" t="s">
         <v>595</v>
@@ -7146,7 +7179,7 @@
         <v>446</v>
       </c>
       <c r="D135" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="E135" t="s">
         <v>596</v>
@@ -7155,7 +7188,7 @@
         <v>746</v>
       </c>
       <c r="G135" t="s">
-        <v>922</v>
+        <v>912</v>
       </c>
       <c r="I135" t="s">
         <v>763</v>
@@ -7181,7 +7214,7 @@
         <v>447</v>
       </c>
       <c r="D136" t="s">
-        <v>923</v>
+        <v>913</v>
       </c>
       <c r="E136" t="s">
         <v>597</v>
@@ -7190,7 +7223,7 @@
         <v>747</v>
       </c>
       <c r="G136" t="s">
-        <v>924</v>
+        <v>914</v>
       </c>
       <c r="K136" t="s">
         <v>763</v>
@@ -7210,7 +7243,7 @@
         <v>448</v>
       </c>
       <c r="D137" t="s">
-        <v>925</v>
+        <v>915</v>
       </c>
       <c r="E137" t="s">
         <v>598</v>
@@ -7219,7 +7252,7 @@
         <v>748</v>
       </c>
       <c r="G137" t="s">
-        <v>926</v>
+        <v>916</v>
       </c>
       <c r="J137" t="s">
         <v>763</v>
@@ -7291,7 +7324,7 @@
         <v>451</v>
       </c>
       <c r="D140" t="s">
-        <v>927</v>
+        <v>917</v>
       </c>
       <c r="E140" t="s">
         <v>601</v>
@@ -7300,7 +7333,7 @@
         <v>751</v>
       </c>
       <c r="G140" t="s">
-        <v>928</v>
+        <v>918</v>
       </c>
       <c r="K140" t="s">
         <v>763</v>
@@ -7320,7 +7353,7 @@
         <v>452</v>
       </c>
       <c r="D141" t="s">
-        <v>929</v>
+        <v>919</v>
       </c>
       <c r="E141" t="s">
         <v>602</v>
@@ -7329,7 +7362,7 @@
         <v>752</v>
       </c>
       <c r="G141" t="s">
-        <v>930</v>
+        <v>920</v>
       </c>
       <c r="H141" t="s">
         <v>763</v>
@@ -7375,7 +7408,7 @@
         <v>454</v>
       </c>
       <c r="D143" t="s">
-        <v>931</v>
+        <v>951</v>
       </c>
       <c r="E143" t="s">
         <v>604</v>
@@ -7384,7 +7417,7 @@
         <v>754</v>
       </c>
       <c r="G143" t="s">
-        <v>932</v>
+        <v>921</v>
       </c>
       <c r="K143" t="s">
         <v>763</v>
@@ -7459,7 +7492,7 @@
         <v>457</v>
       </c>
       <c r="D146" t="s">
-        <v>933</v>
+        <v>922</v>
       </c>
       <c r="E146" t="s">
         <v>607</v>
@@ -7468,7 +7501,7 @@
         <v>757</v>
       </c>
       <c r="G146" t="s">
-        <v>934</v>
+        <v>923</v>
       </c>
       <c r="K146" t="s">
         <v>763</v>
@@ -7488,7 +7521,7 @@
         <v>458</v>
       </c>
       <c r="D147" t="s">
-        <v>948</v>
+        <v>935</v>
       </c>
       <c r="E147" t="s">
         <v>608</v>
@@ -7497,7 +7530,7 @@
         <v>758</v>
       </c>
       <c r="G147" t="s">
-        <v>949</v>
+        <v>936</v>
       </c>
       <c r="K147" t="s">
         <v>763</v>
@@ -7517,7 +7550,7 @@
         <v>459</v>
       </c>
       <c r="D148" t="s">
-        <v>935</v>
+        <v>924</v>
       </c>
       <c r="E148" t="s">
         <v>609</v>
@@ -7526,7 +7559,7 @@
         <v>759</v>
       </c>
       <c r="G148" t="s">
-        <v>936</v>
+        <v>925</v>
       </c>
       <c r="K148" t="s">
         <v>763</v>
@@ -7558,7 +7591,7 @@
         <v>760</v>
       </c>
       <c r="G149" t="s">
-        <v>937</v>
+        <v>926</v>
       </c>
       <c r="K149" t="s">
         <v>763</v>
@@ -7587,7 +7620,7 @@
         <v>761</v>
       </c>
       <c r="G150" t="s">
-        <v>947</v>
+        <v>934</v>
       </c>
       <c r="K150" t="s">
         <v>763</v>
@@ -7607,7 +7640,7 @@
         <v>462</v>
       </c>
       <c r="D151" t="s">
-        <v>938</v>
+        <v>952</v>
       </c>
       <c r="E151" t="s">
         <v>612</v>
@@ -7616,7 +7649,7 @@
         <v>762</v>
       </c>
       <c r="G151" t="s">
-        <v>939</v>
+        <v>953</v>
       </c>
       <c r="K151" t="s">
         <v>763</v>

</xml_diff>